<commit_message>
Modifcata la tesi e nuovo tentativo fallito di far funzionare latex. Alla tesi si sono aggiunti i capitolo 3 e 4.
</commit_message>
<xml_diff>
--- a/Dataset/DatasetVuoto.xlsx
+++ b/Dataset/DatasetVuoto.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\39393\Google Drive\Universita'\Tesi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\39393\Documents\Git\TheaterAnalysis\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1339,7 +1339,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1447,22 +1447,16 @@
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="C2" s="4">
-        <v>0.2</v>
-      </c>
       <c r="D2" s="4" t="str">
         <f>+IF(NOT(B2+C2=100%),"KO","OK")</f>
-        <v>OK</v>
+        <v>KO</v>
       </c>
       <c r="M2" s="4" t="str">
         <f>+IF(NOT(SUM(E2:L2)=100%),"KO","OK")</f>
         <v>KO</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
@@ -1475,7 +1469,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -1514,7 +1508,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>17</v>
       </c>
@@ -1527,7 +1521,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
@@ -1540,7 +1534,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
@@ -1553,7 +1547,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="10" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
@@ -1566,7 +1560,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" ht="120" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
@@ -1592,7 +1586,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
@@ -1605,7 +1599,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="14" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>24</v>
       </c>
@@ -1631,7 +1625,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="16" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>26</v>
       </c>
@@ -1644,7 +1638,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>27</v>
       </c>
@@ -1657,7 +1651,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>28</v>
       </c>
@@ -1670,7 +1664,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>29</v>
       </c>
@@ -1683,7 +1677,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>30</v>
       </c>
@@ -1696,7 +1690,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>31</v>
       </c>
@@ -1709,7 +1703,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>32</v>
       </c>
@@ -1722,7 +1716,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>33</v>
       </c>
@@ -1735,7 +1729,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>34</v>
       </c>
@@ -1748,7 +1742,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>35</v>
       </c>
@@ -1761,7 +1755,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>36</v>
       </c>
@@ -1774,7 +1768,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="150" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="270" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>37</v>
       </c>
@@ -1787,7 +1781,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>38</v>
       </c>
@@ -1800,7 +1794,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>39</v>
       </c>
@@ -1813,7 +1807,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>40</v>
       </c>
@@ -1826,7 +1820,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>41</v>
       </c>
@@ -1839,7 +1833,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>42</v>
       </c>
@@ -1852,7 +1846,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>43</v>
       </c>
@@ -1865,7 +1859,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>44</v>
       </c>
@@ -1878,7 +1872,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>45</v>
       </c>
@@ -1891,7 +1885,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>46</v>
       </c>
@@ -1904,7 +1898,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" ht="165" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>47</v>
       </c>
@@ -1917,7 +1911,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>48</v>
       </c>
@@ -1930,7 +1924,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>49</v>
       </c>
@@ -1943,7 +1937,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>50</v>
       </c>
@@ -1956,7 +1950,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>51</v>
       </c>
@@ -1969,7 +1963,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>52</v>
       </c>
@@ -1982,7 +1976,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>53</v>
       </c>
@@ -1995,7 +1989,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>54</v>
       </c>
@@ -2008,7 +2002,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>55</v>
       </c>
@@ -2021,7 +2015,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>56</v>
       </c>
@@ -2034,7 +2028,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>57</v>
       </c>
@@ -2047,7 +2041,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>58</v>
       </c>
@@ -2060,7 +2054,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>59</v>
       </c>
@@ -2073,7 +2067,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>60</v>
       </c>
@@ -2086,7 +2080,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="51" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>61</v>
       </c>
@@ -2099,7 +2093,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>62</v>
       </c>
@@ -2112,7 +2106,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>63</v>
       </c>
@@ -2125,7 +2119,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>64</v>
       </c>
@@ -2138,7 +2132,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>65</v>
       </c>
@@ -2151,7 +2145,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>66</v>
       </c>
@@ -2164,7 +2158,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>67</v>
       </c>
@@ -2177,7 +2171,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="58" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>68</v>
       </c>
@@ -2190,7 +2184,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>69</v>
       </c>
@@ -2203,7 +2197,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" ht="150" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>70</v>
       </c>
@@ -2216,7 +2210,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="61" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>71</v>
       </c>
@@ -2229,7 +2223,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="62" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>72</v>
       </c>
@@ -2242,7 +2236,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>73</v>
       </c>
@@ -2255,7 +2249,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="64" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>74</v>
       </c>
@@ -2268,7 +2262,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="65" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>75</v>
       </c>
@@ -2281,7 +2275,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="66" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>76</v>
       </c>
@@ -2294,7 +2288,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="67" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>34</v>
       </c>
@@ -2307,7 +2301,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="68" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>35</v>
       </c>
@@ -2320,7 +2314,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="69" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>77</v>
       </c>
@@ -2333,7 +2327,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="70" spans="1:13" ht="150" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" ht="270" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>37</v>
       </c>
@@ -2346,7 +2340,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="71" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>78</v>
       </c>
@@ -2359,7 +2353,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>79</v>
       </c>
@@ -2372,7 +2366,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>80</v>
       </c>
@@ -2385,7 +2379,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="74" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>81</v>
       </c>
@@ -2398,7 +2392,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>82</v>
       </c>
@@ -2411,7 +2405,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="76" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>83</v>
       </c>
@@ -2424,7 +2418,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="77" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>84</v>
       </c>
@@ -2437,7 +2431,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>85</v>
       </c>
@@ -2450,7 +2444,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="79" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>86</v>
       </c>
@@ -2463,7 +2457,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>87</v>
       </c>
@@ -2476,7 +2470,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="81" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>88</v>
       </c>
@@ -2489,7 +2483,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>89</v>
       </c>
@@ -2502,7 +2496,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>90</v>
       </c>
@@ -2515,7 +2509,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>91</v>
       </c>
@@ -2528,7 +2522,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>92</v>
       </c>
@@ -2541,7 +2535,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>93</v>
       </c>
@@ -2554,7 +2548,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="87" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>94</v>
       </c>
@@ -2567,7 +2561,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>95</v>
       </c>
@@ -2580,7 +2574,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="89" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>96</v>
       </c>
@@ -2593,7 +2587,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="90" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>38</v>
       </c>
@@ -2606,7 +2600,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="91" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>97</v>
       </c>
@@ -2619,7 +2613,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="92" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>98</v>
       </c>
@@ -2632,7 +2626,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="93" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>99</v>
       </c>
@@ -2645,7 +2639,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="94" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>100</v>
       </c>
@@ -2658,7 +2652,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="95" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>101</v>
       </c>
@@ -2671,7 +2665,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="96" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13" ht="150" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>102</v>
       </c>
@@ -2684,7 +2678,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="97" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:13" ht="150" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>103</v>
       </c>
@@ -2697,7 +2691,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="98" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>104</v>
       </c>
@@ -2710,7 +2704,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="99" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>105</v>
       </c>
@@ -2723,7 +2717,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="100" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:13" ht="165" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>106</v>
       </c>
@@ -2736,7 +2730,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>107</v>
       </c>
@@ -2749,7 +2743,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="102" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>108</v>
       </c>
@@ -2762,7 +2756,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>109</v>
       </c>
@@ -2775,7 +2769,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>110</v>
       </c>
@@ -2788,7 +2782,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>111</v>
       </c>
@@ -2801,7 +2795,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="106" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>112</v>
       </c>
@@ -2814,7 +2808,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="107" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>113</v>
       </c>
@@ -2827,7 +2821,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="108" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>114</v>
       </c>
@@ -2840,7 +2834,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="109" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>115</v>
       </c>
@@ -2853,7 +2847,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="110" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>116</v>
       </c>
@@ -2866,7 +2860,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="111" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:13" ht="195" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>117</v>
       </c>
@@ -2879,7 +2873,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>118</v>
       </c>
@@ -2892,7 +2886,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>119</v>
       </c>
@@ -2905,7 +2899,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="114" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>120</v>
       </c>
@@ -2918,7 +2912,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="115" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>121</v>
       </c>
@@ -2931,7 +2925,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>122</v>
       </c>
@@ -2944,7 +2938,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="117" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>123</v>
       </c>
@@ -2957,7 +2951,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>124</v>
       </c>
@@ -2970,7 +2964,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="119" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>125</v>
       </c>
@@ -2983,7 +2977,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="120" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>126</v>
       </c>
@@ -2996,7 +2990,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="121" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>127</v>
       </c>
@@ -3009,7 +3003,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="122" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>128</v>
       </c>
@@ -3022,7 +3016,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>129</v>
       </c>
@@ -3035,7 +3029,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="124" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>130</v>
       </c>
@@ -3048,7 +3042,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="125" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:13" ht="165" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>131</v>
       </c>
@@ -3061,7 +3055,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>132</v>
       </c>
@@ -3074,7 +3068,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="127" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>133</v>
       </c>
@@ -3100,7 +3094,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>135</v>
       </c>
@@ -3113,7 +3107,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="130" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>136</v>
       </c>
@@ -3126,7 +3120,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="131" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>137</v>
       </c>
@@ -3139,7 +3133,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="132" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>138</v>
       </c>
@@ -3152,7 +3146,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="133" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:13" ht="150" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>139</v>
       </c>
@@ -3165,7 +3159,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="134" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>140</v>
       </c>
@@ -3204,7 +3198,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="137" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:13" ht="240" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>143</v>
       </c>
@@ -3217,7 +3211,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>144</v>
       </c>
@@ -3256,7 +3250,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>146</v>
       </c>
@@ -3282,7 +3276,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
         <v>147</v>
       </c>
@@ -3308,7 +3302,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
         <v>149</v>
       </c>
@@ -3321,7 +3315,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>150</v>
       </c>
@@ -3334,7 +3328,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="147" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>153</v>
       </c>
@@ -3347,7 +3341,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
         <v>154</v>
       </c>
@@ -3360,7 +3354,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="149" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>155</v>
       </c>
@@ -3373,7 +3367,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="150" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>156</v>
       </c>
@@ -3386,7 +3380,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="151" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:13" ht="180" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>157</v>
       </c>
@@ -3399,7 +3393,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="152" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
         <v>158</v>
       </c>
@@ -3412,7 +3406,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="153" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>159</v>
       </c>
@@ -3425,7 +3419,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="154" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
         <v>160</v>
       </c>
@@ -3438,7 +3432,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="155" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
         <v>161</v>
       </c>
@@ -3451,7 +3445,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="156" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
         <v>162</v>
       </c>
@@ -3464,7 +3458,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
         <v>163</v>
       </c>
@@ -3477,7 +3471,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="158" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
         <v>164</v>
       </c>
@@ -3490,7 +3484,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="159" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
         <v>165</v>
       </c>
@@ -3503,7 +3497,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="160" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
         <v>166</v>
       </c>
@@ -3516,7 +3510,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="161" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
         <v>167</v>
       </c>
@@ -3529,7 +3523,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
         <v>168</v>
       </c>
@@ -3555,7 +3549,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="164" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
         <v>170</v>
       </c>
@@ -3568,7 +3562,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
         <v>171</v>
       </c>
@@ -3581,7 +3575,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
         <v>172</v>
       </c>
@@ -3594,7 +3588,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="167" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:13" ht="240" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
         <v>173</v>
       </c>
@@ -3607,7 +3601,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="168" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
         <v>174</v>
       </c>
@@ -3620,7 +3614,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="169" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
         <v>175</v>
       </c>
@@ -3633,7 +3627,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="170" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:13" ht="180" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
         <v>176</v>
       </c>
@@ -3646,7 +3640,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="171" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
         <v>177</v>
       </c>
@@ -3659,7 +3653,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="172" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
         <v>178</v>
       </c>
@@ -3672,7 +3666,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="173" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
         <v>179</v>
       </c>
@@ -3685,7 +3679,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="174" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
         <v>180</v>
       </c>
@@ -3698,7 +3692,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="175" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
         <v>181</v>
       </c>
@@ -3711,7 +3705,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="176" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
         <v>182</v>
       </c>
@@ -3724,7 +3718,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="177" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
         <v>183</v>
       </c>
@@ -3737,7 +3731,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="178" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
         <v>184</v>
       </c>
@@ -3763,7 +3757,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="180" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
         <v>186</v>
       </c>
@@ -3776,7 +3770,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="181" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
         <v>187</v>
       </c>
@@ -3789,7 +3783,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="182" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
         <v>188</v>
       </c>
@@ -3828,7 +3822,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="185" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
         <v>191</v>
       </c>
@@ -3841,7 +3835,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="186" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
         <v>192</v>
       </c>
@@ -3854,7 +3848,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="187" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
         <v>193</v>
       </c>
@@ -3867,7 +3861,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="188" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
         <v>194</v>
       </c>
@@ -3880,7 +3874,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="189" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:13" ht="165" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
         <v>195</v>
       </c>
@@ -3893,7 +3887,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="190" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
         <v>196</v>
       </c>
@@ -3906,7 +3900,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="191" spans="1:13" ht="135" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:13" ht="270" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
         <v>197</v>
       </c>
@@ -3919,7 +3913,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="192" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:13" ht="150" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
         <v>198</v>
       </c>
@@ -3932,7 +3926,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="193" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
         <v>199</v>
       </c>
@@ -3945,7 +3939,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="194" spans="1:13" ht="135" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:13" ht="300" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
         <v>200</v>
       </c>
@@ -3958,7 +3952,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="195" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
         <v>201</v>
       </c>
@@ -3971,7 +3965,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="196" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
         <v>202</v>
       </c>
@@ -3984,7 +3978,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="197" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:13" ht="210" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
         <v>203</v>
       </c>
@@ -3997,7 +3991,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="198" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:13" ht="150" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
         <v>204</v>
       </c>
@@ -4010,7 +4004,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="199" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:13" ht="150" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
         <v>205</v>
       </c>
@@ -4023,7 +4017,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="200" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
         <v>206</v>
       </c>
@@ -4036,7 +4030,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="201" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:13" ht="225" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
         <v>207</v>
       </c>
@@ -4049,7 +4043,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="202" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:13" ht="150" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
         <v>208</v>
       </c>
@@ -4062,7 +4056,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="203" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
         <v>209</v>
       </c>
@@ -4075,7 +4069,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="204" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
         <v>210</v>
       </c>
@@ -4088,7 +4082,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="205" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
         <v>211</v>
       </c>
@@ -4101,7 +4095,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="206" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
         <v>212</v>
       </c>
@@ -4114,7 +4108,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="207" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
         <v>213</v>
       </c>
@@ -4127,7 +4121,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="208" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
         <v>214</v>
       </c>
@@ -4140,7 +4134,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="209" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:13" ht="210" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
         <v>215</v>
       </c>
@@ -4153,7 +4147,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="210" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
         <v>216</v>
       </c>
@@ -4166,7 +4160,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="211" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
         <v>217</v>
       </c>
@@ -4179,7 +4173,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="212" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
         <v>218</v>
       </c>
@@ -4192,7 +4186,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="213" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A213" s="2" t="s">
         <v>219</v>
       </c>
@@ -4205,7 +4199,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="214" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
         <v>220</v>
       </c>
@@ -4218,7 +4212,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="215" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
         <v>221</v>
       </c>
@@ -4231,7 +4225,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="216" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
         <v>222</v>
       </c>
@@ -4244,7 +4238,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="217" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
         <v>223</v>
       </c>
@@ -4257,7 +4251,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="218" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
         <v>224</v>
       </c>
@@ -4270,7 +4264,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="219" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
         <v>225</v>
       </c>
@@ -4283,7 +4277,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="220" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
         <v>226</v>
       </c>
@@ -4296,7 +4290,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="221" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
         <v>227</v>
       </c>
@@ -4309,7 +4303,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="222" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
         <v>228</v>
       </c>
@@ -4322,7 +4316,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="223" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
         <v>229</v>
       </c>
@@ -4335,7 +4329,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="224" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
         <v>230</v>
       </c>
@@ -4348,7 +4342,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="225" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A225" s="2" t="s">
         <v>231</v>
       </c>
@@ -4361,7 +4355,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="226" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
         <v>232</v>
       </c>
@@ -4374,7 +4368,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="227" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A227" s="2" t="s">
         <v>233</v>
       </c>
@@ -4387,7 +4381,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="228" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
         <v>234</v>
       </c>
@@ -4400,7 +4394,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="229" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A229" s="2" t="s">
         <v>235</v>
       </c>
@@ -4413,7 +4407,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="230" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
         <v>236</v>
       </c>
@@ -4426,7 +4420,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="231" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
         <v>237</v>
       </c>
@@ -4439,7 +4433,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="232" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A232" s="2" t="s">
         <v>238</v>
       </c>
@@ -4452,7 +4446,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="233" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A233" s="2" t="s">
         <v>239</v>
       </c>
@@ -4465,7 +4459,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="234" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A234" s="2" t="s">
         <v>240</v>
       </c>
@@ -4478,7 +4472,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="235" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A235" s="2" t="s">
         <v>241</v>
       </c>
@@ -4491,7 +4485,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="236" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A236" s="2" t="s">
         <v>242</v>
       </c>
@@ -4504,7 +4498,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="237" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A237" s="2" t="s">
         <v>233</v>
       </c>
@@ -4517,7 +4511,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="238" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:13" ht="225" x14ac:dyDescent="0.25">
       <c r="A238" s="2" t="s">
         <v>243</v>
       </c>
@@ -4530,7 +4524,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="239" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A239" s="2" t="s">
         <v>244</v>
       </c>
@@ -4543,7 +4537,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="240" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A240" s="2" t="s">
         <v>244</v>
       </c>
@@ -4556,7 +4550,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="241" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A241" s="2" t="s">
         <v>245</v>
       </c>
@@ -4569,7 +4563,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="242" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A242" s="2" t="s">
         <v>246</v>
       </c>
@@ -4582,7 +4576,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="243" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A243" s="2" t="s">
         <v>247</v>
       </c>
@@ -4595,7 +4589,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="244" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:13" ht="180" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
         <v>248</v>
       </c>
@@ -4608,7 +4602,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="245" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A245" s="2" t="s">
         <v>249</v>
       </c>
@@ -4621,7 +4615,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="246" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A246" s="2" t="s">
         <v>250</v>
       </c>
@@ -4634,7 +4628,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="247" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A247" s="2" t="s">
         <v>251</v>
       </c>
@@ -4647,7 +4641,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="248" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:13" ht="270" x14ac:dyDescent="0.25">
       <c r="A248" s="2" t="s">
         <v>252</v>
       </c>
@@ -4660,7 +4654,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="249" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A249" s="2" t="s">
         <v>253</v>
       </c>
@@ -4673,7 +4667,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="250" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:13" ht="195" x14ac:dyDescent="0.25">
       <c r="A250" s="2" t="s">
         <v>254</v>
       </c>
@@ -4686,7 +4680,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="251" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:13" ht="285" x14ac:dyDescent="0.25">
       <c r="A251" s="2" t="s">
         <v>255</v>
       </c>
@@ -4699,7 +4693,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="252" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A252" s="2" t="s">
         <v>256</v>
       </c>
@@ -4712,7 +4706,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="253" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A253" s="2" t="s">
         <v>257</v>
       </c>
@@ -4725,7 +4719,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="254" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A254" s="2" t="s">
         <v>258</v>
       </c>
@@ -4738,7 +4732,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="255" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A255" s="2" t="s">
         <v>259</v>
       </c>
@@ -4751,7 +4745,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="256" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A256" s="2" t="s">
         <v>260</v>
       </c>
@@ -4764,7 +4758,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="257" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A257" s="2" t="s">
         <v>261</v>
       </c>
@@ -4777,7 +4771,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="258" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A258" s="2" t="s">
         <v>262</v>
       </c>
@@ -4790,7 +4784,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="259" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A259" s="2" t="s">
         <v>263</v>
       </c>
@@ -4803,7 +4797,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="260" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A260" s="2" t="s">
         <v>264</v>
       </c>
@@ -4816,7 +4810,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="261" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A261" s="2" t="s">
         <v>265</v>
       </c>
@@ -4829,7 +4823,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="262" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A262" s="2" t="s">
         <v>266</v>
       </c>
@@ -4842,7 +4836,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="263" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
         <v>267</v>
       </c>
@@ -4855,7 +4849,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="264" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:13" ht="165" x14ac:dyDescent="0.25">
       <c r="A264" s="2" t="s">
         <v>268</v>
       </c>
@@ -4868,7 +4862,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="265" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A265" s="2" t="s">
         <v>269</v>
       </c>
@@ -4881,7 +4875,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="266" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A266" s="2" t="s">
         <v>270</v>
       </c>
@@ -4894,7 +4888,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="267" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A267" s="2" t="s">
         <v>271</v>
       </c>
@@ -4907,7 +4901,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="268" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A268" s="2" t="s">
         <v>272</v>
       </c>
@@ -4920,7 +4914,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="269" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:13" ht="150" x14ac:dyDescent="0.25">
       <c r="A269" s="2" t="s">
         <v>273</v>
       </c>
@@ -4933,7 +4927,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="270" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A270" s="2" t="s">
         <v>274</v>
       </c>
@@ -4946,7 +4940,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="271" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:13" ht="195" x14ac:dyDescent="0.25">
       <c r="A271" s="2" t="s">
         <v>275</v>
       </c>
@@ -4959,7 +4953,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="272" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A272" s="2" t="s">
         <v>276</v>
       </c>
@@ -4972,7 +4966,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="273" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A273" s="2" t="s">
         <v>277</v>
       </c>
@@ -4985,7 +4979,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="274" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A274" s="2" t="s">
         <v>278</v>
       </c>
@@ -4998,7 +4992,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="275" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A275" s="2" t="s">
         <v>279</v>
       </c>
@@ -5011,7 +5005,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="276" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:13" ht="255" x14ac:dyDescent="0.25">
       <c r="A276" s="2" t="s">
         <v>280</v>
       </c>
@@ -5024,7 +5018,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="277" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A277" s="2" t="s">
         <v>281</v>
       </c>
@@ -5037,7 +5031,7 @@
         <v>KO</v>
       </c>
     </row>
-    <row r="278" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A278" s="2" t="s">
         <v>282</v>
       </c>

</xml_diff>